<commit_message>
added Final version of technical document, presentation. also added pairing algorithms description document
</commit_message>
<xml_diff>
--- a/ჯგუფურის სია - გადახედილი.xlsx
+++ b/ჯგუფურის სია - გადახედილი.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA6D12A7-ED8E-4EE1-A1B6-FE3D585DAD0D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="127">
   <si>
     <t>ფბ</t>
   </si>
@@ -367,12 +368,45 @@
   </si>
   <si>
     <t>ხზ მივწერე Giorgi Maisuradze-ს</t>
+  </si>
+  <si>
+    <t>Uridia Daviti</t>
+  </si>
+  <si>
+    <t>Kloyan Manvel</t>
+  </si>
+  <si>
+    <t>Korakhashvili Luka</t>
+  </si>
+  <si>
+    <t>Tsikelashvili Giorgi</t>
+  </si>
+  <si>
+    <t>Makandarashvili Gia</t>
+  </si>
+  <si>
+    <t>Latsabidze Giorgi</t>
+  </si>
+  <si>
+    <t>Mirzashvili Giorgi</t>
+  </si>
+  <si>
+    <t>Sabashvili Irakli</t>
+  </si>
+  <si>
+    <t>Kochladze Guram</t>
+  </si>
+  <si>
+    <t>Shonia Saba</t>
+  </si>
+  <si>
+    <t>Chankvetadze Mariam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,7 +485,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,11 +762,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -743,7 +777,7 @@
     <col min="4" max="4" width="37.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -757,13 +791,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -782,8 +816,17 @@
       <c r="G3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>117</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -802,8 +845,17 @@
       <c r="G4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>118</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -819,8 +871,17 @@
       <c r="G5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>121</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -836,8 +897,17 @@
       <c r="G6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" t="s">
+        <v>120</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -856,8 +926,17 @@
       <c r="G7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -876,8 +955,17 @@
       <c r="G8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
+        <v>123</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -896,8 +984,17 @@
       <c r="G9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" t="s">
+        <v>116</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -913,8 +1010,17 @@
       <c r="G10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" t="s">
+        <v>124</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -930,8 +1036,17 @@
       <c r="G11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11" t="s">
+        <v>125</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -950,8 +1065,17 @@
       <c r="G12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" t="s">
+        <v>119</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -970,8 +1094,17 @@
       <c r="G13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -991,7 +1124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1005,7 +1138,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1419,6 +1552,21 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="J3:J13">
+    <sortCondition ref="J3"/>
+  </sortState>
+  <conditionalFormatting sqref="O3:O13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>